<commit_message>
dataloader implementation now takes a member, refactored, updated unit tests
</commit_message>
<xml_diff>
--- a/src/main/resources/members.xlsx
+++ b/src/main/resources/members.xlsx
@@ -2,15 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a4qt9zz\ee.workspace\TeamGenerator\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13080" windowHeight="3912"/>
   </bookViews>
   <sheets>
     <sheet name="members" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" refMode="R1C1"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="152511" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="107">
   <si>
     <t>jen</t>
   </si>
@@ -334,7 +338,13 @@
     <t>Last_Name</t>
   </si>
   <si>
-    <t>First _Name</t>
+    <t>First_Name</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>age</t>
   </si>
 </sst>
 </file>
@@ -433,7 +443,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -468,7 +478,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -653,439 +663,757 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="D1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="D2">
         <v>2</v>
       </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
       <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="D3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="D5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="D6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="D7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="D8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="D9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="D10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="D11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="D12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="D13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="D14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="D15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="D16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="D17">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="D18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="D19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="D20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="D21">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="D22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="D23">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+      <c r="D24">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+      <c r="D25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+      <c r="D26">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+      <c r="D27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="D28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+      <c r="D29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+      <c r="D30">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+      <c r="D31">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+      <c r="D33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+      <c r="D34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+      <c r="D35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+      <c r="D36">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+      <c r="D37">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+      <c r="D38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+      <c r="D39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+      <c r="D40">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+      <c r="D41">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+      <c r="D42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
+      <c r="D43">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
+      <c r="D44">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+      <c r="D45">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+      <c r="D46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
+      <c r="D47">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+      <c r="D48">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+      <c r="D49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+      <c r="D50">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+      <c r="D51">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
+      <c r="D52">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>102</v>
+      </c>
+      <c r="D53">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>